<commit_message>
Experimentation with TDMA transmission and reception
</commit_message>
<xml_diff>
--- a/parts list/Mouser_order.xlsx
+++ b/parts list/Mouser_order.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="William_telemetry_pickle" sheetId="1" r:id="rId1"/>
@@ -177,12 +177,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -243,13 +249,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -635,7 +642,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,7 +672,7 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -683,7 +690,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -701,7 +708,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -722,7 +729,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
@@ -740,7 +747,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -761,7 +768,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
@@ -797,7 +804,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
@@ -815,7 +822,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">

</xml_diff>